<commit_message>
Adding new kind of graphs & adding a new line for the excel
</commit_message>
<xml_diff>
--- a/plots/alerts_cdb.xlsx
+++ b/plots/alerts_cdb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/VdE/VdE_data_analysis/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="114_{FC3E8DE7-5EA6-476C-A864-D5076C36D9BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{33F5319E-A3DE-45C4-AA4F-F9AD18B0186A}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="114_{051385BF-D3CF-4545-8B77-01216E2E4114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A30A99FA-CE63-4746-9D9A-F8A19423CC7D}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>A1</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>CDB043</t>
+  </si>
+  <si>
+    <t>Bilan</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,27 +488,27 @@
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>-41.024919167173209</v>
+        <v>-31.682522530926871</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2">
-        <v>59.201661087334202</v>
+        <v>32.962910532276332</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2">
-        <v>-58.804851229108991</v>
+        <v>-48.761222212613539</v>
       </c>
       <c r="G2" s="2">
-        <v>297.14003349093531</v>
+        <v>99.521055975372292</v>
       </c>
       <c r="H2" s="2">
-        <v>-123.36814935351219</v>
+        <v>-139.68958475153161</v>
       </c>
       <c r="I2" s="2">
-        <v>-77.563180604068222</v>
+        <v>-69.73951598004804</v>
       </c>
       <c r="J2" s="2">
-        <v>-59.46154215275876</v>
+        <v>-49.440361998596508</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -513,13 +516,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>-25.18073050225528</v>
+        <v>-18.325301969017811</v>
       </c>
       <c r="C3" s="2">
-        <v>-37.662867481820378</v>
+        <v>-28.7133331986164</v>
       </c>
       <c r="D3" s="2">
-        <v>40.119440122447493</v>
+        <v>23.591383137643621</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -533,27 +536,27 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>-84.33004478378821</v>
+        <v>-78.202867617092338</v>
       </c>
       <c r="C4" s="2">
-        <v>-62.362962302739192</v>
+        <v>-52.485894376605437</v>
       </c>
       <c r="D4" s="2">
-        <v>-58.07080272646953</v>
+        <v>-48.006444348933549</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
-        <v>183.9336429656079</v>
+        <v>76.01605949048664</v>
       </c>
       <c r="G4" s="2">
-        <v>108.1288343558282</v>
+        <v>52.987598647125147</v>
       </c>
       <c r="H4" s="2">
-        <v>160.47352314823101</v>
+        <v>69.699348640539739</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2">
-        <v>-14.044398898063299</v>
+        <v>-9.8227828683494014</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -561,23 +564,25 @@
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>-56.687509967179693</v>
+        <v>-46.596465277662588</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
-        <v>-20.62707217626722</v>
+        <v>-14.76669363559925</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
-        <v>-83.771782192410654</v>
-      </c>
-      <c r="G5" s="2"/>
+        <v>-77.48459756252069</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-99.865995160936365</v>
+      </c>
       <c r="H5" s="2">
-        <v>-82.292433034637867</v>
+        <v>-75.599056276928422</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2">
-        <v>152.0772305750215</v>
+        <v>67.279314369178138</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -585,28 +590,28 @@
         <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>-29.258373065837869</v>
+        <v>-21.613501696916959</v>
       </c>
       <c r="C6" s="2">
-        <v>-107.36428990149039</v>
+        <v>-111.4687301192356</v>
       </c>
       <c r="D6" s="2">
-        <v>-23.349176561376439</v>
+        <v>-16.879889436914389</v>
       </c>
       <c r="E6" s="2">
-        <v>183.69422060258671</v>
+        <v>75.954689048688763</v>
       </c>
       <c r="F6" s="2">
-        <v>-69.543543486237255</v>
+        <v>-60.352870592787369</v>
       </c>
       <c r="G6" s="2">
-        <v>9.0527218576523936</v>
+        <v>5.8583673382575974</v>
       </c>
       <c r="H6" s="2">
-        <v>-45.219805724119183</v>
+        <v>-35.497112208929657</v>
       </c>
       <c r="I6" s="2">
-        <v>46.987777166707112</v>
+        <v>27.08324630359084</v>
       </c>
       <c r="J6" s="2"/>
     </row>
@@ -615,27 +620,29 @@
         <v>14</v>
       </c>
       <c r="B7" s="2">
-        <v>-72.2921787856381</v>
+        <v>-63.495560582948038</v>
       </c>
       <c r="C7" s="2">
-        <v>-102.7820541316658</v>
+        <v>-104.2319487500237</v>
       </c>
       <c r="D7" s="2">
-        <v>-61.374964442347483</v>
+        <v>-51.440507320548193</v>
       </c>
       <c r="E7" s="2">
-        <v>-105.44897220446541</v>
+        <v>-108.4023799815524</v>
       </c>
       <c r="F7" s="2">
-        <v>-102.01037783207521</v>
+        <v>-103.04618667897159</v>
       </c>
       <c r="G7" s="2">
-        <v>-106.53388652915611</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>-110.1318309629569</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-100</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2">
-        <v>-74.498876322285568</v>
+        <v>-66.074062166323529</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -643,27 +650,27 @@
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>204.81569253754409</v>
+        <v>81.144740769845072</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
-        <v>-58.27952067223594</v>
+        <v>-48.220590025565073</v>
       </c>
       <c r="E8" s="2">
-        <v>-59.620738730077953</v>
+        <v>-49.605559493861477</v>
       </c>
       <c r="F8" s="2">
-        <v>-60.488582049920339</v>
+        <v>-50.509977827051003</v>
       </c>
       <c r="G8" s="2">
-        <v>357.75973219934491</v>
+        <v>108.7812812751876</v>
       </c>
       <c r="H8" s="2">
-        <v>-69.858280274015641</v>
+        <v>-60.708923490440228</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2">
-        <v>-14.727141845785919</v>
+        <v>-10.32495130526906</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -671,27 +678,27 @@
         <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>-35.034916030694028</v>
+        <v>-26.44493040807787</v>
       </c>
       <c r="C9" s="2">
-        <v>-64.369139661128486</v>
+        <v>-54.635576654565767</v>
       </c>
       <c r="D9" s="2">
-        <v>-65.30275442784901</v>
+        <v>-55.648505178364807</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
-        <v>-2.1123474265019331</v>
+        <v>-1.418217511369148</v>
       </c>
       <c r="G9" s="2">
-        <v>-70.986897529502812</v>
+        <v>-61.993743382999469</v>
       </c>
       <c r="H9" s="2">
-        <v>-78.055743884158218</v>
+        <v>-70.33815179557314</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2">
-        <v>-85.087541636416319</v>
+        <v>-79.18344267642901</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -699,21 +706,21 @@
         <v>17</v>
       </c>
       <c r="B10" s="2">
-        <v>82.398945255146401</v>
+        <v>43.095801532699163</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
-        <v>-42.578208970167161</v>
+        <v>-33.080500916282382</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <v>-38.049823431907171</v>
+        <v>-29.051191284092351</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2">
-        <v>61.019201139808821</v>
+        <v>33.803853616183922</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -721,24 +728,24 @@
         <v>18</v>
       </c>
       <c r="B11" s="2">
-        <v>-17.055664794420299</v>
+        <v>-12.05584468197825</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
-        <v>-39.276622600990322</v>
+        <v>-30.128961194669991</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
-        <v>-13.62357456031337</v>
+        <v>-9.5144525527172696</v>
       </c>
       <c r="G11" s="2">
-        <v>-27.598631422775309</v>
+        <v>-20.263210546206349</v>
       </c>
       <c r="H11" s="2">
-        <v>-35.062189054726367</v>
+        <v>-26.46824092765598</v>
       </c>
       <c r="I11" s="2">
-        <v>17.252824491070971</v>
+        <v>10.876388267778241</v>
       </c>
       <c r="J11" s="2"/>
     </row>
@@ -747,28 +754,60 @@
         <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>32.260947274352098</v>
+        <v>19.419042495965581</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
-        <v>20.485829959514181</v>
+        <v>12.784234461849421</v>
       </c>
       <c r="E12" s="2">
-        <v>-44.858294468947179</v>
+        <v>-35.163435452921327</v>
       </c>
       <c r="F12" s="2">
-        <v>9.4830537487162001</v>
+        <v>6.1283185840707954</v>
       </c>
       <c r="G12" s="2">
-        <v>-0.47543581616481778</v>
+        <v>-0.31746031746031739</v>
       </c>
       <c r="H12" s="2">
-        <v>45.661157024793418</v>
+        <v>26.41960549910344</v>
       </c>
       <c r="I12" s="2">
-        <v>-9.0066559946077938</v>
+        <v>-6.1902831663674744</v>
       </c>
       <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-169.38207490470049</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-3351.5969524299312</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-1146.4077416878761</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-3036.7466324437169</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-2520.9576606668788</v>
+      </c>
+      <c r="G13" s="2">
+        <v>527.16561371143644</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-3299.1082223560052</v>
+      </c>
+      <c r="I13" s="2">
+        <v>-3790.841674027015</v>
+      </c>
+      <c r="J13" s="2">
+        <v>-1347.826128814796</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:J12">

</xml_diff>

<commit_message>
Rename files + correction alerts + plot
</commit_message>
<xml_diff>
--- a/plots/alerts_cdb.xlsx
+++ b/plots/alerts_cdb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/VdE/VdE_data_analysis/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="114_{A12F11F3-6D73-4152-80F4-9D26CC79F2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FEA8CC4-6F44-4FBE-87BA-FE79AC721A2A}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_387955BE8760D36607DA2511595ED87656CD2798" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5B9C7E8-5D31-450F-A565-A326AD188BAD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,7 +244,7 @@
     <t>CDB043</t>
   </si>
   <si>
-    <t>Bilan en Watt</t>
+    <t>Bilan en kWh</t>
   </si>
 </sst>
 </file>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AD10" sqref="AD10:AJ10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BF3" sqref="BF3:BL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,13 +811,13 @@
         <v>63</v>
       </c>
       <c r="B2">
-        <v>114.8783746020259</v>
+        <v>43.252249734683943</v>
       </c>
       <c r="C2">
-        <v>11.84340852450635</v>
+        <v>-25.437727650329101</v>
       </c>
       <c r="D2">
-        <v>46.296793729090851</v>
+        <v>-2.4688041806060941</v>
       </c>
       <c r="E2">
         <v>-31.682522530926871</v>
@@ -831,15 +831,6 @@
       <c r="H2">
         <v>-28.714658288274091</v>
       </c>
-      <c r="I2">
-        <v>-100.0111208217596</v>
-      </c>
-      <c r="N2">
-        <v>-100.0731478166947</v>
-      </c>
-      <c r="O2">
-        <v>-100.046137963145</v>
-      </c>
       <c r="P2">
         <v>30.27183086742226</v>
       </c>
@@ -861,18 +852,6 @@
       <c r="V2">
         <v>-27.397291495194288</v>
       </c>
-      <c r="W2">
-        <v>-100.0100968441844</v>
-      </c>
-      <c r="AA2">
-        <v>-100.09600435954221</v>
-      </c>
-      <c r="AB2">
-        <v>-100.0452319283346</v>
-      </c>
-      <c r="AC2">
-        <v>-100.0326518765759</v>
-      </c>
       <c r="AD2">
         <v>20.037668020672552</v>
       </c>
@@ -915,27 +894,6 @@
       <c r="AQ2">
         <v>4.0771260570361418</v>
       </c>
-      <c r="AR2">
-        <v>-271.976136658391</v>
-      </c>
-      <c r="AS2">
-        <v>86616.89494133211</v>
-      </c>
-      <c r="AT2">
-        <v>717.87783394550229</v>
-      </c>
-      <c r="AU2">
-        <v>-139.68958475153161</v>
-      </c>
-      <c r="AV2">
-        <v>-100.21614427630441</v>
-      </c>
-      <c r="AW2">
-        <v>-100.12668408084031</v>
-      </c>
-      <c r="AX2">
-        <v>-101.24822832708669</v>
-      </c>
       <c r="AY2">
         <v>-72.146527455872246</v>
       </c>
@@ -958,13 +916,13 @@
         <v>-64.859750877951427</v>
       </c>
       <c r="BF2">
-        <v>50.527072566866551</v>
+        <v>0.35138171124437168</v>
       </c>
       <c r="BG2">
-        <v>8.7101893345842409</v>
+        <v>-27.526540443610511</v>
       </c>
       <c r="BH2">
-        <v>-20.24632979813406</v>
+        <v>-46.83088653208938</v>
       </c>
       <c r="BI2">
         <v>-49.440361998596508</v>
@@ -984,13 +942,13 @@
         <v>64</v>
       </c>
       <c r="B3">
-        <v>14.483919201196169</v>
+        <v>-23.677387199202549</v>
       </c>
       <c r="C3">
-        <v>-17.164136703250911</v>
+        <v>-44.776091135500607</v>
       </c>
       <c r="D3">
-        <v>0.4166312388402269</v>
+        <v>-33.055579174106512</v>
       </c>
       <c r="E3">
         <v>-18.325301969017811</v>
@@ -1005,13 +963,13 @@
         <v>4.4257426298444154</v>
       </c>
       <c r="I3">
-        <v>20.17780360177025</v>
+        <v>-19.8814642654865</v>
       </c>
       <c r="J3">
-        <v>11.091057217155511</v>
+        <v>-25.939295188562991</v>
       </c>
       <c r="K3">
-        <v>-1.12159911160465</v>
+        <v>-34.081066074403097</v>
       </c>
       <c r="L3">
         <v>-28.7133331986164</v>
@@ -1035,16 +993,16 @@
         <v>-12.63031097850263</v>
       </c>
       <c r="S3">
-        <v>23.591383137643621</v>
+        <v>-17.60574457490425</v>
       </c>
       <c r="T3">
-        <v>43.506140552794818</v>
+        <v>-4.3292396314701262</v>
       </c>
       <c r="U3">
-        <v>51.009167186433807</v>
+        <v>0.6727781242892189</v>
       </c>
       <c r="V3">
-        <v>49.366317398826318</v>
+        <v>-0.42245506744911848</v>
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.3">
@@ -1052,13 +1010,13 @@
         <v>65</v>
       </c>
       <c r="B4">
-        <v>13.32559072576387</v>
+        <v>-24.449606182824091</v>
       </c>
       <c r="C4">
-        <v>-11.34140112372793</v>
+        <v>-40.894267415818618</v>
       </c>
       <c r="D4">
-        <v>-15.1807619781423</v>
+        <v>-43.453841318761533</v>
       </c>
       <c r="E4">
         <v>-78.202867617092338</v>
@@ -1073,13 +1031,13 @@
         <v>8.6480558233470184</v>
       </c>
       <c r="I4">
-        <v>35.839383772237412</v>
+        <v>-9.440410818508397</v>
       </c>
       <c r="J4">
-        <v>27.844772871520529</v>
+        <v>-14.77015141898632</v>
       </c>
       <c r="K4">
-        <v>-24.69401028834972</v>
+        <v>-49.796006858899823</v>
       </c>
       <c r="L4">
         <v>-52.485894376605437</v>
@@ -1178,13 +1136,13 @@
         <v>80.53392294755956</v>
       </c>
       <c r="BF4">
-        <v>76.370415303487789</v>
+        <v>17.58027686899187</v>
       </c>
       <c r="BG4">
-        <v>90.601932689353333</v>
+        <v>27.06795512623556</v>
       </c>
       <c r="BH4">
-        <v>127.2653227127787</v>
+        <v>51.510215141852477</v>
       </c>
       <c r="BI4">
         <v>-9.8227828683494014</v>
@@ -1204,13 +1162,13 @@
         <v>66</v>
       </c>
       <c r="B5">
-        <v>39.252378835844461</v>
+        <v>-7.1650807761036894</v>
       </c>
       <c r="C5">
-        <v>1.400692840646655</v>
+        <v>-32.399538106235561</v>
       </c>
       <c r="D5">
-        <v>-14.22709142974024</v>
+        <v>-42.818060953160163</v>
       </c>
       <c r="E5">
         <v>-46.596465277662588</v>
@@ -1309,13 +1267,13 @@
         <v>-25.92827475003417</v>
       </c>
       <c r="BF5">
-        <v>78.360369919262411</v>
+        <v>18.90691327950827</v>
       </c>
       <c r="BG5">
-        <v>102.447718705871</v>
+        <v>34.965145803913977</v>
       </c>
       <c r="BH5">
-        <v>98.798463466530904</v>
+        <v>32.532308977687258</v>
       </c>
       <c r="BI5">
         <v>67.279314369178138</v>
@@ -1335,13 +1293,13 @@
         <v>67</v>
       </c>
       <c r="B6">
-        <v>47.264295255741793</v>
+        <v>-1.8238031628388049</v>
       </c>
       <c r="C6">
-        <v>32.37214363438521</v>
+        <v>-11.7519042437432</v>
       </c>
       <c r="D6">
-        <v>60.104011887072787</v>
+        <v>6.736007924715202</v>
       </c>
       <c r="E6">
         <v>-21.613501696916959</v>
@@ -1355,27 +1313,6 @@
       <c r="H6">
         <v>-17.839197543025051</v>
       </c>
-      <c r="I6">
-        <v>-149.62984278128019</v>
-      </c>
-      <c r="J6">
-        <v>-133.6864982341755</v>
-      </c>
-      <c r="K6">
-        <v>-129.92097724170199</v>
-      </c>
-      <c r="L6">
-        <v>-111.4687301192356</v>
-      </c>
-      <c r="M6">
-        <v>-114.0363402021722</v>
-      </c>
-      <c r="N6">
-        <v>-112.3075654754673</v>
-      </c>
-      <c r="O6">
-        <v>-117.0015077430586</v>
-      </c>
       <c r="P6">
         <v>-36.041927815650517</v>
       </c>
@@ -1398,13 +1335,13 @@
         <v>-14.36870070427544</v>
       </c>
       <c r="W6">
-        <v>19.328723048637809</v>
+        <v>-20.44751796757479</v>
       </c>
       <c r="X6">
-        <v>9.637956221980664</v>
+        <v>-26.90802918534623</v>
       </c>
       <c r="Y6">
-        <v>9.378292939936772</v>
+        <v>-27.081138040042141</v>
       </c>
       <c r="Z6">
         <v>75.954689048688763</v>
@@ -1491,16 +1428,16 @@
         <v>4.1180323778034298</v>
       </c>
       <c r="BB6">
-        <v>27.08324630359084</v>
+        <v>-15.2778357976061</v>
       </c>
       <c r="BC6">
-        <v>19.783393501805069</v>
+        <v>-20.144404332129959</v>
       </c>
       <c r="BD6">
-        <v>27.742316811333939</v>
+        <v>-14.838455459110699</v>
       </c>
       <c r="BE6">
-        <v>44.924705234960363</v>
+        <v>-3.3835298433597569</v>
       </c>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.3">
@@ -1508,13 +1445,13 @@
         <v>68</v>
       </c>
       <c r="B7">
-        <v>23.079029019894151</v>
+        <v>-17.947313986737239</v>
       </c>
       <c r="C7">
-        <v>17.097392597869248</v>
+        <v>-21.9350716014205</v>
       </c>
       <c r="D7">
-        <v>0.42768950902793929</v>
+        <v>-33.048206993981367</v>
       </c>
       <c r="E7">
         <v>-63.495560582948038</v>
@@ -1528,27 +1465,6 @@
       <c r="H7">
         <v>-28.237552178114779</v>
       </c>
-      <c r="I7">
-        <v>-109.029161433585</v>
-      </c>
-      <c r="J7">
-        <v>-105.4093735937879</v>
-      </c>
-      <c r="K7">
-        <v>-104.6989438473408</v>
-      </c>
-      <c r="L7">
-        <v>-104.2319487500237</v>
-      </c>
-      <c r="M7">
-        <v>-108.8968592456563</v>
-      </c>
-      <c r="N7">
-        <v>-108.9477436522714</v>
-      </c>
-      <c r="O7">
-        <v>-110.8270033059476</v>
-      </c>
       <c r="P7">
         <v>-23.217831991831819</v>
       </c>
@@ -1570,77 +1486,14 @@
       <c r="V7">
         <v>-22.40250539011177</v>
       </c>
-      <c r="W7">
-        <v>-107.36214576382351</v>
-      </c>
-      <c r="X7">
-        <v>-108.42379425907041</v>
-      </c>
-      <c r="Y7">
-        <v>-109.7551444169661</v>
-      </c>
-      <c r="Z7">
-        <v>-108.4023799815524</v>
-      </c>
-      <c r="AA7">
-        <v>-110.9878085476944</v>
-      </c>
-      <c r="AB7">
-        <v>-109.71137298155141</v>
-      </c>
-      <c r="AC7">
-        <v>-107.996265735881</v>
-      </c>
-      <c r="AD7">
-        <v>-109.71638380578069</v>
-      </c>
-      <c r="AE7">
-        <v>-110.5931509415916</v>
-      </c>
-      <c r="AF7">
-        <v>-110.6539621412694</v>
-      </c>
-      <c r="AG7">
-        <v>-103.04618667897159</v>
-      </c>
-      <c r="AH7">
-        <v>-102.4428499140156</v>
-      </c>
-      <c r="AI7">
-        <v>-104.42956094111599</v>
-      </c>
-      <c r="AJ7">
-        <v>-107.2800970814302</v>
-      </c>
-      <c r="AK7">
-        <v>-118.40084009465259</v>
-      </c>
-      <c r="AL7">
-        <v>-114.83677507773891</v>
-      </c>
-      <c r="AM7">
-        <v>-121.50168153238781</v>
-      </c>
-      <c r="AN7">
-        <v>-110.1318309629569</v>
-      </c>
-      <c r="AO7">
-        <v>-112.5102793885082</v>
-      </c>
-      <c r="AP7">
-        <v>-111.2693903378598</v>
-      </c>
-      <c r="AQ7">
-        <v>-115.7816177532666</v>
-      </c>
       <c r="BF7">
-        <v>-29.582706182160969</v>
+        <v>-53.055137454773977</v>
       </c>
       <c r="BG7">
-        <v>-30.294393907729471</v>
+        <v>-53.52959593848631</v>
       </c>
       <c r="BH7">
-        <v>-39.485012566605818</v>
+        <v>-59.656675044403883</v>
       </c>
       <c r="BI7">
         <v>-66.074062166323529</v>
@@ -1660,13 +1513,13 @@
         <v>69</v>
       </c>
       <c r="B8">
-        <v>89.479824596693092</v>
+        <v>26.319883064462051</v>
       </c>
       <c r="C8">
-        <v>91.367008324367191</v>
+        <v>27.57800554957813</v>
       </c>
       <c r="D8">
-        <v>122.1809268902918</v>
+        <v>48.1206179268612</v>
       </c>
       <c r="E8">
         <v>81.144740769845072</v>
@@ -1702,13 +1555,13 @@
         <v>-16.10896945120929</v>
       </c>
       <c r="W8">
-        <v>64.496384169888728</v>
+        <v>9.6642561132591549</v>
       </c>
       <c r="X8">
-        <v>40.222461835310128</v>
+        <v>-6.5183587764599134</v>
       </c>
       <c r="Y8">
-        <v>-12.004677955136421</v>
+        <v>-41.336451970090948</v>
       </c>
       <c r="Z8">
         <v>-49.605559493861477</v>
@@ -1786,13 +1639,13 @@
         <v>-35.034195241737777</v>
       </c>
       <c r="BF8">
-        <v>32.690204825503891</v>
+        <v>-11.53986344966407</v>
       </c>
       <c r="BG8">
-        <v>1.733327418261092</v>
+        <v>-32.17778172115927</v>
       </c>
       <c r="BH8">
-        <v>20.221213840045358</v>
+        <v>-19.85252410663643</v>
       </c>
       <c r="BI8">
         <v>-10.32495130526906</v>
@@ -1812,13 +1665,13 @@
         <v>70</v>
       </c>
       <c r="B9">
-        <v>79.026132100260526</v>
+        <v>19.35075473350701</v>
       </c>
       <c r="C9">
-        <v>99.630859193561776</v>
+        <v>33.087239462374527</v>
       </c>
       <c r="D9">
-        <v>97.126256959129947</v>
+        <v>31.41750463941997</v>
       </c>
       <c r="E9">
         <v>-26.44493040807787</v>
@@ -1833,13 +1686,13 @@
         <v>-5.8644964649225138</v>
       </c>
       <c r="I9">
-        <v>80.058528266051681</v>
+        <v>20.039018844034459</v>
       </c>
       <c r="J9">
-        <v>85.927950939930952</v>
+        <v>23.9519672932873</v>
       </c>
       <c r="K9">
-        <v>91.719650195945079</v>
+        <v>27.813100130630058</v>
       </c>
       <c r="L9">
         <v>-54.635576654565767</v>
@@ -1938,13 +1791,13 @@
         <v>-36.965521889764702</v>
       </c>
       <c r="BF9">
-        <v>-25.76711838670904</v>
+        <v>-50.511412257806029</v>
       </c>
       <c r="BG9">
-        <v>-42.706041365436597</v>
+        <v>-61.804027576957729</v>
       </c>
       <c r="BH9">
-        <v>-35.070928247689693</v>
+        <v>-56.713952165126457</v>
       </c>
       <c r="BI9">
         <v>-79.18344267642901</v>
@@ -1964,13 +1817,13 @@
         <v>71</v>
       </c>
       <c r="B10">
-        <v>38.736895516036391</v>
+        <v>-7.5087363226424104</v>
       </c>
       <c r="C10">
-        <v>0.49611606348704013</v>
+        <v>-33.00258929100864</v>
       </c>
       <c r="D10">
-        <v>-25.765448135090001</v>
+        <v>-50.510298756726669</v>
       </c>
       <c r="E10">
         <v>43.095801532699163</v>
@@ -2027,13 +1880,13 @@
         <v>-4.1485633024806852</v>
       </c>
       <c r="BF10">
-        <v>77.611120050220165</v>
+        <v>18.407413366813451</v>
       </c>
       <c r="BG10">
-        <v>101.03414017341041</v>
+        <v>34.02276011560695</v>
       </c>
       <c r="BH10">
-        <v>109.6629771925811</v>
+        <v>39.77531812838739</v>
       </c>
       <c r="BI10">
         <v>33.803853616183922</v>
@@ -2053,13 +1906,13 @@
         <v>72</v>
       </c>
       <c r="B11">
-        <v>34.526015813442363</v>
+        <v>-10.31598945770509</v>
       </c>
       <c r="C11">
-        <v>41.776323214084186</v>
+        <v>-5.4824511906105373</v>
       </c>
       <c r="D11">
-        <v>51.874702113011693</v>
+        <v>1.249801408674466</v>
       </c>
       <c r="E11">
         <v>-12.05584468197825</v>
@@ -2167,16 +2020,16 @@
         <v>-0.71207310960014403</v>
       </c>
       <c r="BB11">
-        <v>10.876388267778241</v>
+        <v>-26.082407821481169</v>
       </c>
       <c r="BC11">
-        <v>39.614614614614617</v>
+        <v>-6.9235902569235872</v>
       </c>
       <c r="BD11">
-        <v>46.743219164521868</v>
+        <v>-2.1711872236520851</v>
       </c>
       <c r="BE11">
-        <v>60.823175336319203</v>
+        <v>7.2154502242127938</v>
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.3">
@@ -2184,13 +2037,13 @@
         <v>73</v>
       </c>
       <c r="B12">
-        <v>57.564423595042634</v>
+        <v>5.0429490633617524</v>
       </c>
       <c r="C12">
-        <v>57.579410839710633</v>
+        <v>5.0529405598070936</v>
       </c>
       <c r="D12">
-        <v>62.379580891846253</v>
+        <v>8.2530539278975041</v>
       </c>
       <c r="E12">
         <v>19.419042495965581</v>
@@ -2226,13 +2079,13 @@
         <v>-10.02706623792513</v>
       </c>
       <c r="W12">
-        <v>-57.765220561429103</v>
+        <v>-71.843480374286059</v>
       </c>
       <c r="X12">
-        <v>-20.799863271235701</v>
+        <v>-47.199908847490462</v>
       </c>
       <c r="Y12">
-        <v>2.2260718925941858</v>
+        <v>-31.849285404937209</v>
       </c>
       <c r="Z12">
         <v>-35.163435452921327</v>
@@ -2298,16 +2151,16 @@
         <v>-24.391520544360109</v>
       </c>
       <c r="AU12">
-        <v>26.41960549910344</v>
+        <v>-15.72026300059771</v>
       </c>
       <c r="AV12">
-        <v>7.6488989756486578</v>
+        <v>-28.23406734956756</v>
       </c>
       <c r="AW12">
-        <v>36.718616201404352</v>
+        <v>-8.8542558657304351</v>
       </c>
       <c r="AX12">
-        <v>49.219458152885501</v>
+        <v>-0.52036123140966928</v>
       </c>
       <c r="AY12">
         <v>-69.39649980210288</v>
@@ -2336,197 +2189,197 @@
         <v>74</v>
       </c>
       <c r="B13">
-        <v>2066.0790046758789</v>
+        <v>227.96812499999999</v>
       </c>
       <c r="C13">
-        <v>1090.813377594628</v>
+        <v>62.112916666666663</v>
       </c>
       <c r="D13">
-        <v>1589.946598925766</v>
+        <v>21.20366666666667</v>
       </c>
       <c r="E13">
-        <v>-169.38207490470049</v>
+        <v>-318.38474999999988</v>
       </c>
       <c r="F13">
-        <v>122.2110754192902</v>
+        <v>-210.94916666666671</v>
       </c>
       <c r="G13">
-        <v>-238.98161044973739</v>
+        <v>-126.3341666666667</v>
       </c>
       <c r="H13">
-        <v>-179.8878755019941</v>
+        <v>-34.415335393772907</v>
       </c>
       <c r="I13">
-        <v>-630.37719166694842</v>
+        <v>26.952354166666641</v>
       </c>
       <c r="J13">
-        <v>-733.52738160391004</v>
+        <v>-33.801958333333317</v>
       </c>
       <c r="K13">
-        <v>-726.08468122524198</v>
+        <v>-76.913083333333333</v>
       </c>
       <c r="L13">
-        <v>-3351.5969524299312</v>
+        <v>-99.588124999999991</v>
       </c>
       <c r="M13">
-        <v>-2896.6422563079632</v>
+        <v>-85.73566666666666</v>
       </c>
       <c r="N13">
-        <v>-3360.8832853400031</v>
+        <v>-71.307791666666688</v>
       </c>
       <c r="O13">
-        <v>-2517.1481930920158</v>
+        <v>-15.030927083333349</v>
       </c>
       <c r="P13">
-        <v>563.33140572342393</v>
+        <v>1.2889791666666379</v>
       </c>
       <c r="Q13">
-        <v>594.58484640937786</v>
+        <v>-170.33937499999999</v>
       </c>
       <c r="R13">
-        <v>218.51620800495809</v>
+        <v>-247.55083333333329</v>
       </c>
       <c r="S13">
-        <v>-1146.4077416878761</v>
+        <v>-316.52962500000001</v>
       </c>
       <c r="T13">
-        <v>-661.20777145996635</v>
+        <v>-295.58808333333337</v>
       </c>
       <c r="U13">
-        <v>-370.56458045743392</v>
+        <v>-169.3099</v>
       </c>
       <c r="V13">
-        <v>-99.856383431658756</v>
+        <v>-28.445566666666661</v>
       </c>
       <c r="W13">
-        <v>-1832.76426689043</v>
+        <v>6.2335208333333352</v>
       </c>
       <c r="X13">
-        <v>-1746.2411253619071</v>
+        <v>-8.5939999999999941</v>
       </c>
       <c r="Y13">
-        <v>-1759.22318885397</v>
+        <v>-15.28466666666667</v>
       </c>
       <c r="Z13">
-        <v>-3036.7466324437169</v>
+        <v>-24.885000000000002</v>
       </c>
       <c r="AA13">
-        <v>-3222.3083346181938</v>
+        <v>-17.87908333333333</v>
       </c>
       <c r="AB13">
-        <v>-2403.8979826440318</v>
+        <v>-2.0436250000000018</v>
       </c>
       <c r="AC13">
-        <v>-2064.5847945548858</v>
+        <v>6.5324583333333344</v>
       </c>
       <c r="AD13">
-        <v>-549.5730395276596</v>
+        <v>-13.73114583333335</v>
       </c>
       <c r="AE13">
-        <v>-1450.438364793139</v>
+        <v>-123.245125</v>
       </c>
       <c r="AF13">
-        <v>-2004.681409269605</v>
+        <v>-196.1596666666666</v>
       </c>
       <c r="AG13">
-        <v>-2520.9576606668788</v>
+        <v>-185.44450000000001</v>
       </c>
       <c r="AH13">
-        <v>-2089.8928017179578</v>
+        <v>-137.3410833333333</v>
       </c>
       <c r="AI13">
-        <v>-2401.07661346755</v>
+        <v>-116.1660833333333</v>
       </c>
       <c r="AJ13">
-        <v>-2149.9482843601968</v>
+        <v>-61.337217803030313</v>
       </c>
       <c r="AK13">
-        <v>-1152.999919273037</v>
+        <v>-61.819657012195172</v>
       </c>
       <c r="AL13">
-        <v>-1276.068251007106</v>
+        <v>-142.48065931372551</v>
       </c>
       <c r="AM13">
-        <v>-651.63602503769891</v>
+        <v>-145.23031666666671</v>
       </c>
       <c r="AN13">
-        <v>527.16561371143644</v>
+        <v>-121.94275</v>
       </c>
       <c r="AO13">
-        <v>-1263.05059999695</v>
+        <v>-183.6809166666666</v>
       </c>
       <c r="AP13">
-        <v>-1062.007305681122</v>
+        <v>-118.0817361111111</v>
       </c>
       <c r="AQ13">
-        <v>-796.57517944202846</v>
+        <v>-3.7462749999999998</v>
       </c>
       <c r="AR13">
-        <v>-2357.0492133994749</v>
+        <v>-26.219791666666669</v>
       </c>
       <c r="AS13">
-        <v>-2495.8367251908371</v>
+        <v>-60.007375000000003</v>
       </c>
       <c r="AT13">
-        <v>-3383.5284513060551</v>
+        <v>-82.906583333333344</v>
       </c>
       <c r="AU13">
-        <v>-3299.1082223560052</v>
+        <v>-123.3715</v>
       </c>
       <c r="AV13">
-        <v>-1655.3616322208291</v>
+        <v>-84.723416666666665</v>
       </c>
       <c r="AW13">
-        <v>-1190.0129599834211</v>
+        <v>-35.331500000000013</v>
       </c>
       <c r="AX13">
-        <v>-1249.534090028802</v>
+        <v>5.6622083333333437</v>
       </c>
       <c r="AY13">
-        <v>-3006.899379549543</v>
+        <v>-63.74647916666671</v>
       </c>
       <c r="AZ13">
-        <v>-2886.9474969033981</v>
+        <v>-65.493208333333328</v>
       </c>
       <c r="BA13">
-        <v>-2503.7175912307721</v>
+        <v>-70.894750000000016</v>
       </c>
       <c r="BB13">
-        <v>-3790.841674027015</v>
+        <v>-98.911633333333384</v>
       </c>
       <c r="BC13">
-        <v>-2328.678312287811</v>
+        <v>-83.691333333333318</v>
       </c>
       <c r="BD13">
-        <v>-1685.073659110783</v>
+        <v>-53.405583333333347</v>
       </c>
       <c r="BE13">
-        <v>-1606.8474086653141</v>
+        <v>-43.870229166666682</v>
       </c>
       <c r="BF13">
-        <v>285.57452387513001</v>
+        <v>-34.887395833333358</v>
       </c>
       <c r="BG13">
-        <v>127.48918290752989</v>
+        <v>-103.70399999999999</v>
       </c>
       <c r="BH13">
-        <v>278.44749851947131</v>
+        <v>-145.3764166666667</v>
       </c>
       <c r="BI13">
-        <v>-1347.826128814796</v>
+        <v>-243.53691666666671</v>
       </c>
       <c r="BJ13">
-        <v>-1140.950196727468</v>
+        <v>-190.82149999999999</v>
       </c>
       <c r="BK13">
-        <v>-967.84924766779761</v>
+        <v>-113.7895833333333</v>
       </c>
       <c r="BL13">
-        <v>-1126.5766488430211</v>
+        <v>-70.565645833333335</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:BL13">
+  <conditionalFormatting sqref="A1:BL13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Adding new methods for plotting
</commit_message>
<xml_diff>
--- a/plots/alerts_cdb.xlsx
+++ b/plots/alerts_cdb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/brice_petit_ulb_be/Documents/Ulb/PhD/VdE/VdE_data_analysis/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_387955BE8760D36607DA2511595ED87656CD2798" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D5B9C7E8-5D31-450F-A565-A326AD188BAD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{F64C5ED5-37C0-4660-99B2-72A4794C6001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="1440" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BF3" sqref="BF3:BL3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adaption plot average + check dates
</commit_message>
<xml_diff>
--- a/plots/alerts_cdb.xlsx
+++ b/plots/alerts_cdb.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,20 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -216,7 +229,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,10 +303,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,9 +596,9 @@
       <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:134" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:134">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:134" s="3" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>106.58805530080591</v>
       </c>
     </row>
-    <row r="3" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:134" s="3" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>1.5549572410022781</v>
       </c>
     </row>
-    <row r="4" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:134" s="3" customFormat="1">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -1671,7 +1680,7 @@
         <v>65.865917526521145</v>
       </c>
     </row>
-    <row r="5" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:134" s="3" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>50.228255829086322</v>
       </c>
     </row>
-    <row r="6" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:134" s="3" customFormat="1">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -2272,7 +2281,7 @@
         <v>16.488256693283709</v>
       </c>
     </row>
-    <row r="7" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:134" s="3" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -2565,7 +2574,7 @@
         <v>17.913477853378179</v>
       </c>
     </row>
-    <row r="8" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:134" s="3" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2855,7 +2864,7 @@
         <v>-16.96038138073164</v>
       </c>
     </row>
-    <row r="9" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:134" s="3" customFormat="1">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>-0.831000171742729</v>
       </c>
     </row>
-    <row r="10" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:134" s="3" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -3357,7 +3366,7 @@
         <v>-26.388114008869731</v>
       </c>
     </row>
-    <row r="11" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:134" s="3" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -3629,7 +3638,7 @@
         <v>-17.92322829240134</v>
       </c>
     </row>
-    <row r="12" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:134" s="3" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -3796,7 +3805,7 @@
         <v>25.778597179358179</v>
       </c>
     </row>
-    <row r="13" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:134" s="3" customFormat="1">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -3906,7 +3915,7 @@
         <v>1.8306873334888769</v>
       </c>
     </row>
-    <row r="14" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:134" s="3" customFormat="1">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3995,7 +4004,7 @@
         <v>3.522160950480012</v>
       </c>
     </row>
-    <row r="15" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:134" s="3" customFormat="1">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -4084,7 +4093,7 @@
         <v>61.843567269616031</v>
       </c>
     </row>
-    <row r="16" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:134" s="3" customFormat="1">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -4173,7 +4182,7 @@
         <v>56.710926485508587</v>
       </c>
     </row>
-    <row r="17" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:134" s="3" customFormat="1">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -4313,7 +4322,7 @@
         <v>131.3197559745868</v>
       </c>
     </row>
-    <row r="18" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:134" s="3" customFormat="1">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -4399,7 +4408,7 @@
         <v>108.3922564636121</v>
       </c>
     </row>
-    <row r="19" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:134" s="3" customFormat="1">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -4479,7 +4488,7 @@
         <v>-25.986866743499679</v>
       </c>
     </row>
-    <row r="20" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:134" s="3" customFormat="1">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
@@ -4667,7 +4676,7 @@
         <v>35.795829139261727</v>
       </c>
     </row>
-    <row r="21" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:134" s="3" customFormat="1">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -4756,7 +4765,7 @@
         <v>42.551004939859808</v>
       </c>
     </row>
-    <row r="22" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:134" s="3" customFormat="1">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
@@ -4863,7 +4872,7 @@
         <v>-33.998769930602627</v>
       </c>
     </row>
-    <row r="23" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:134" s="3" customFormat="1">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -4952,7 +4961,7 @@
         <v>14.43291993761267</v>
       </c>
     </row>
-    <row r="24" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:134" s="3" customFormat="1">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -4999,7 +5008,7 @@
         <v>126.087789884988</v>
       </c>
     </row>
-    <row r="25" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:134" s="3" customFormat="1">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -5046,7 +5055,7 @@
         <v>132.41435796773939</v>
       </c>
     </row>
-    <row r="26" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:134" s="3" customFormat="1">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
@@ -5156,7 +5165,7 @@
         <v>-16.578002880498421</v>
       </c>
     </row>
-    <row r="27" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:134" s="3" customFormat="1">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
@@ -5245,7 +5254,7 @@
         <v>42.54003899762894</v>
       </c>
     </row>
-    <row r="28" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:134" s="3" customFormat="1">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -5259,7 +5268,7 @@
         <v>-46.833015669152267</v>
       </c>
     </row>
-    <row r="29" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:134" s="3" customFormat="1">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
@@ -5348,7 +5357,7 @@
         <v>13.094882062090241</v>
       </c>
     </row>
-    <row r="30" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:134" s="3" customFormat="1">
       <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
@@ -5437,7 +5446,7 @@
         <v>76.835984537427919</v>
       </c>
     </row>
-    <row r="31" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:134" s="3" customFormat="1">
       <c r="A31" s="2" t="s">
         <v>54</v>
       </c>
@@ -5505,7 +5514,7 @@
         <v>-75.155348519394835</v>
       </c>
     </row>
-    <row r="32" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:134" s="3" customFormat="1">
       <c r="A32" s="2" t="s">
         <v>55</v>
       </c>
@@ -5594,7 +5603,7 @@
         <v>44.65326263882109</v>
       </c>
     </row>
-    <row r="33" spans="1:134" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:134" s="3" customFormat="1">
       <c r="A33" s="2" t="s">
         <v>56</v>
       </c>

</xml_diff>